<commit_message>
commit message: Data Corrected, New Visuals Added, and LLM-RLHF Notebook Included
</commit_message>
<xml_diff>
--- a/Yeni Veri/Q-2-calibrated-damped.xlsx
+++ b/Yeni Veri/Q-2-calibrated-damped.xlsx
@@ -478,415 +478,415 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>20190808014</v>
+        <v>20210808035</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>advanced modern legal system civil engineering military engineering like gregorian calendar divided powers known division powers 3 parties consuls senate assemblies mention conflict interests example senators forbidden trade influences gains trading terms theaters having great open - air settings tales gods love etc romanian theater stories closed realistic shows acted makes theater influence democracy</t>
+          <t>introduce calendars calculate days 1 year 12 tables rule empire</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" t="n">
         <v>11</v>
       </c>
       <c r="F2" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G2" t="n">
         <v>16</v>
       </c>
       <c r="H2" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>20190808021</v>
+        <v>20220808013</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>main battlefield surgeries bound books 12 tables julian calendar aqueducts roman bridges roads highways newspapers welfare concrete working mathematical philosophical astronomical improvements worked military building law improvements thinker builder</t>
+          <t>introduce laws apply laws units like consuls assemblies senate law s 12 tables</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G3" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>20190808035</v>
+        <v>20220808706</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>roads highways geometry military engineering science changes life</t>
+          <t>checks balances vetoes separation powers term limits</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G4" t="n">
         <v>13</v>
       </c>
       <c r="H4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>20200808003</v>
-      </c>
-      <c r="B5" t="inlineStr"/>
+        <v>20220808063</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>introduced twelve tables guilty proven guilty prisons firstly equal ruler</t>
+        </is>
+      </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G5" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>20200808008</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>achieved civil army engineering republic government system fundamentals modern legal systems road trade web europe rule medittarenean hundreds years seeking answers questions nature developing theories philosophies developed science philosophy improved tools armies cities laws government system divine power rulers</t>
-        </is>
-      </c>
+        <v>20220808019</v>
+      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
         <v>12</v>
       </c>
-      <c r="G6" t="n">
-        <v>16</v>
-      </c>
       <c r="H6" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>20200808015</v>
+        <v>20220808617</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>contribute law world rules strict</t>
+          <t>lawyer jury juries prison</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
         <v>8</v>
       </c>
       <c r="G7" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>19.42554093119887</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>20200808020</v>
+        <v>20220808029</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>great war government didn t choose king choose consuls senator assemblies instead king roads highways roads economy great table set laws invented newspaper aches julien calendar difference science understand nature tool thought philosophy trough government</t>
+          <t>twelve tables rome</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E8" t="n">
         <v>9</v>
       </c>
       <c r="F8" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G8" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H8" t="n">
-        <v>10.36639229629243</v>
+        <v>16.63646437226229</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>20200808026</v>
+        <v>20220808014</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>good engineering predictable improving invention practical information improve themself military invented arches</t>
+          <t>government closed consulates senate assemblies</t>
         </is>
       </c>
       <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G9" t="n">
         <v>11</v>
       </c>
-      <c r="D9" t="n">
-        <v>5</v>
-      </c>
-      <c r="E9" t="n">
-        <v>11</v>
-      </c>
-      <c r="F9" t="n">
-        <v>8</v>
-      </c>
-      <c r="G9" t="n">
-        <v>14</v>
-      </c>
       <c r="H9" t="n">
-        <v>9.166844975490456</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>20200808033</v>
+        <v>20210808014</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>- theater pop ancient greece like birthplace theater focused mythological ethical themes roman theater included greek theater focused comedy drama - political pop ancient greece city - state system state governance monarchy republic empire military engineering discipline - cultural discipline contributed philosophy democracy mythology contributed law engineering architecture military</t>
+          <t>lawyer improved laws way works society introduced lawyer jury system</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" t="n">
         <v>13</v>
       </c>
       <c r="F10" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" t="n">
         <v>16</v>
       </c>
       <c r="H10" t="n">
-        <v>14.53620564394753</v>
+        <v>6.403980448147268</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>20200808038</v>
+        <v>20220808059</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>battlefield surgery tables newspaper julian calendar approach science differently science practical tool explain nature coherent theory usually worked legal systems government better philosophy astronomy</t>
+          <t>revolt plebs modern judgment system like today 12 tables system 2 consuls 1 assembly 1 senate 2 consuls makes wrong decision reject decision</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D11" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E11" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" t="n">
         <v>11</v>
-      </c>
-      <c r="F11" t="n">
-        <v>9</v>
       </c>
       <c r="G11" t="n">
         <v>15</v>
       </c>
       <c r="H11" t="n">
-        <v>11.0149448084382</v>
+        <v>16.64106024942392</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>20200808045</v>
+        <v>20220808006</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>wants biggest empire world science example developed highways roads battlefield surgery science understand predict nature think main difference</t>
+          <t>introduced modern legal concepts assemblies sent conceals distribution power important arrested innocent proofing guilty</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D12" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E12" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G12" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H12" t="n">
-        <v>11.57348231172666</v>
+        <v>17.68423940367263</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>20200808062</v>
+        <v>20230808077</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>roads important achievement roads army faster travel help economy making faster travel traders</t>
+          <t>introduce 12 table law introduce council prison introduce compass roads highways</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D13" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G13" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H13" t="n">
-        <v>7.9820775316589</v>
+        <v>6.776575144492681</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>20200808063</v>
+        <v>20220808504</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>theaters argued theaters</t>
+          <t>early civilizations ruled kings priests laws punishments following laws corpus juries included modern legal concepts liquor accused innocent proven guilty duo judgment punishments based precedent rulings previous judges juries</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D14" t="n">
         <v>5</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G14" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>6.423781785392084</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>20200808072</v>
+        <v>20190808014</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3 kind governments consuls senate assemble theater comedy theater religion myth</t>
+          <t>corpus juries committed modern legal concepts like accused innocent proven guilty judgement punishments based previous judgement eventually found concept lawyer ones called lawyer translators traders venice eventually person advices criminal cases division powers technique modern legal system 3 parties consuls senate assemblies mention conflict interests</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D15" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G15" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H15" t="n">
-        <v>8</v>
+        <v>4.781525478804272</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>20200808504</v>
+        <v>20210808605</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>theatre roman s theatre judge government people loves topics t drama realistic problems</t>
+          <t>roman law codes equality law presumption innocence presumption innocence property rights contracts obligations torts liability testamentary succession legal procedures civil rights</t>
         </is>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F16" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G16" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -894,217 +894,217 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>20200808505</v>
+        <v>20230808611</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>theatre harsh topic judge government people works</t>
+          <t>accuse innocent proven guilty create twelve table</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G17" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>17.28021851760843</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>20200808805</v>
+        <v>20200808033</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>- julian calender - aqueducts - concrete roads highways</t>
+          <t>- citizenship rights - inheritance - modern government - julian calender - welfare - newspaper - 12 tables</t>
         </is>
       </c>
       <c r="C18" t="n">
         <v>8</v>
       </c>
       <c r="D18" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F18" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G18" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H18" t="n">
-        <v>9.071825334213523</v>
+        <v>8.200158534665304</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>20210808005</v>
+        <v>20210808025</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>inventions tables concrete newspaper julian calendar welfare biggest difference policy democracy rules laws punishments laws following laws consuls senator assemblies</t>
+          <t>lawyer prison jury said accused innocent proven guilty important humans</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D19" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E19" t="n">
+        <v>8</v>
+      </c>
+      <c r="F19" t="n">
+        <v>8</v>
+      </c>
+      <c r="G19" t="n">
         <v>13</v>
       </c>
-      <c r="F19" t="n">
-        <v>11</v>
-      </c>
-      <c r="G19" t="n">
-        <v>17</v>
-      </c>
       <c r="H19" t="n">
-        <v>15.65723551894306</v>
+        <v>19.42935946896376</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>20210808006</v>
+        <v>20220808610</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>copy</t>
+          <t>jury voting diversity power innocent proved guilty</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D20" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G20" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>19.36084173181549</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20210808012</v>
+        <v>20220808050</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>created legal concepts concrete newspaper highways bound books</t>
+          <t>laws</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E21" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F21" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G21" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" t="n">
-        <v>11.24797277055028</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>20210808014</v>
+        <v>20210808012</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>improved social engineering theatre laws social language translators difference theatre roman theatre people critique politics</t>
+          <t>console senate assemblies</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F22" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G22" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H22" t="n">
-        <v>12.34276448105694</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>20210808016</v>
+        <v>20210808608</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>observation support theories theories observation roma doesn t like science practical tool explain nature</t>
+          <t>introduce modern world power division concept concept includes counselors senate assembles</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E23" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F23" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G23" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H23" t="n">
-        <v>4.950612053039338</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>20210808017</v>
+        <v>20230808621</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>actually bit similar example roman theater theater verry roman theater seating arrangement people sitting accordingly social status theater sit want played theater entertainment teacher instilled democracy ideology people theater bit political theater entertaining places invented new thing like newspaper</t>
+          <t>find jury system people judge collect jury decide common ideas find temporary prison guilty people publish 12 rules judge system example people innocent find proof guilty</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D24" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F24" t="n">
         <v>10</v>
@@ -1113,32 +1113,28 @@
         <v>15</v>
       </c>
       <c r="H24" t="n">
-        <v>10</v>
+        <v>16.63915826818473</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>20210808018</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>theaters</t>
-        </is>
-      </c>
+        <v>20220808601</v>
+      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -1146,317 +1142,315 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>20210808021</v>
+        <v>20220808071</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>science medicine military tool science tool science explain nature calculated days year found days mouth produced tool medicine</t>
+          <t>calculate observation theory</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
+        <v>5</v>
+      </c>
+      <c r="E26" t="n">
         <v>6</v>
       </c>
-      <c r="E26" t="n">
-        <v>9</v>
-      </c>
       <c r="F26" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G26" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H26" t="n">
-        <v>8.756565682047944</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>20210808022</v>
+        <v>20220808069</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>wanted strictly deductive proofs based stated axioms thought systematically systematic science military donot science science invented newspaper roads concrete bound books roman arches welfare theater public concept protocol theater concept protocol public julian calendar didnot</t>
+          <t>12 table judgement punishment based precedent concept lawyer jury prison help meet</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D27" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E27" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F27" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G27" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H27" t="n">
-        <v>10.40057974159549</v>
+        <v>5.411092793454904</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>20210808025</v>
+        <v>20230808609</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>practical tools observation predict power division means power emperor 3 groups consuls sent assemblies consuls choose government 2 people consuls vote person sent t trade engage bank conflict inflict</t>
+          <t>1 consuls heads state putting laws power veto 2 consuls select commanding army 2 senate selected populace 3 assembles assemble power pass law heading people tribes</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E28" t="n">
         <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G28" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H28" t="n">
-        <v>11.95481941645728</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>20210808033</v>
+        <v>20220808023</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>bang world roman government division power s conduction thought new invented julian calendar</t>
+          <t>introduced division power division power means divide power state instead concentrating king priests introduced principle states guilty guilt proven</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D29" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E29" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F29" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G29" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H29" t="n">
-        <v>10</v>
+        <v>18.54821865781198</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>20210808035</v>
+        <v>20220808016</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>modern government consuls senate assembly better civil engineering military engineering good highways roads good connection empire</t>
+          <t>introduced consumer sent assemblies consumer powerful people command army 2 people wanted avoid despotism assemblies pass law existed tribes senate legal power</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
         <v>7</v>
       </c>
       <c r="E30" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G30" t="n">
         <v>15</v>
       </c>
       <c r="H30" t="n">
-        <v>11.67949509124324</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>20210808038</v>
+        <v>20230808070</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>achieved democracy ended monarchy bring representative division power system power people right vote stated legal system 12 tablets laws actions crimes develop julian later gregorian calendar pretty accurate compare sum biggest legal government system science</t>
+          <t>introduced consuls powerful organization government senate assemblies power pass law</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E31" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F31" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G31" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H31" t="n">
-        <v>18.58815530714798</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>20210808042</v>
+        <v>20230808010</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>legal law democracy table consented newspaper</t>
+          <t>introduced main concepts lawyers jury prison lawyers advisors given accused person help lawyers worked translators occasions jury group people helps making final decision trials prison accused person stays trial</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D32" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E32" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F32" t="n">
         <v>9</v>
       </c>
       <c r="G32" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H32" t="n">
-        <v>10</v>
+        <v>17.68042086590775</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>20210808044</v>
+        <v>20210808018</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>gained democracy successful divided 3 power consult senator assemblies science technology technology military science understand nature</t>
+          <t>senator judges court</t>
         </is>
       </c>
       <c r="C33" t="n">
+        <v>8</v>
+      </c>
+      <c r="D33" t="n">
+        <v>7</v>
+      </c>
+      <c r="E33" t="n">
+        <v>7</v>
+      </c>
+      <c r="F33" t="n">
+        <v>8</v>
+      </c>
+      <c r="G33" t="n">
         <v>13</v>
       </c>
-      <c r="D33" t="n">
-        <v>7</v>
-      </c>
-      <c r="E33" t="n">
-        <v>10</v>
-      </c>
-      <c r="F33" t="n">
-        <v>8</v>
-      </c>
-      <c r="G33" t="n">
-        <v>15</v>
-      </c>
       <c r="H33" t="n">
-        <v>10.35039452563315</v>
+        <v>19.19118088847508</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>20210808048</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>excellent road calender laws conflict interest avoid monarchy wanted strictly deductive way based axioms</t>
-        </is>
-      </c>
+        <v>20230808602</v>
+      </c>
+      <c r="B34" t="inlineStr"/>
       <c r="C34" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G34" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H34" t="n">
-        <v>9.365339334071345</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>20210808056</v>
+        <v>20210808022</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>took care civil engineering military engineering improve technology created highways big cities division power consult senate assemblies justice system orderly strict established 12 tables rules</t>
+          <t>concepts lawyer jury prison accused innocent proven guilty roman twelve table establish laws understand division power</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D35" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E35" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F35" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G35" t="n">
         <v>16</v>
       </c>
-      <c r="H35" t="inlineStr"/>
+      <c r="H35" t="n">
+        <v>4.356110399223707</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>20210808061</v>
+        <v>20200808026</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>established calendar established modern legal system good travel roadways highways good travel network grew economy science practical tool understand explain nature</t>
+          <t>12 table rules presented innocent guilty</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D36" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E36" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F36" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G36" t="n">
         <v>15</v>
       </c>
       <c r="H36" t="n">
-        <v>12.76796982122946</v>
+        <v>17.56324084454585</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>20210808062</v>
+        <v>20220808076</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>copy</t>
+          <t>di vi son power conflict ct interest sai d innocent unti l qui lay wi ll proof</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1466,13 +1460,13 @@
         <v>3</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G37" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -1480,71 +1474,71 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>20210808065</v>
+        <v>20220808048</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>engineering</t>
+          <t>lawyer prison person arrest trial jury decision person punished consult assemble</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D38" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F38" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G38" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H38" t="n">
-        <v>4.436270405500238</v>
+        <v>18.96063938351617</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>20210808066</v>
+        <v>20210808062</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>systematic approach natural sciences greek strictly deductive science br style color rob 36 36 36</t>
+          <t>roman s modern legal notions concepts lawyer venice story jury verdict prison person arrest trial division power instead king 3 parties guard despotism consuls senate assemblies</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D39" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F39" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G39" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H39" t="n">
-        <v>7.287850352340034</v>
+        <v>16.69163909016325</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>20210808076</v>
+        <v>20220808607</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>want learn earlier wonder possible live earth</t>
+          <t>legal concepts written law legal science public law private law 12 tables democracy guy consuls senate etc</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
@@ -1558,309 +1552,311 @@
       <c r="G40" t="n">
         <v>0</v>
       </c>
-      <c r="H40" t="n">
-        <v>0</v>
-      </c>
+      <c r="H40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>20210808604</v>
+        <v>20210808615</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>aqueducts civil engineering military engineering highways want solve problems especially war want finding mean</t>
+          <t>roman law legal system ancient rome including legal developments spanning thousand years jurisprudence</t>
         </is>
       </c>
       <c r="C41" t="n">
+        <v>8</v>
+      </c>
+      <c r="D41" t="n">
+        <v>8</v>
+      </c>
+      <c r="E41" t="n">
         <v>15</v>
       </c>
-      <c r="D41" t="n">
-        <v>6</v>
-      </c>
-      <c r="E41" t="n">
-        <v>10</v>
-      </c>
       <c r="F41" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G41" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H41" t="n">
-        <v>9.431522320692968</v>
+        <v>0.9928876546915879</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>20210808605</v>
+        <v>20220808024</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>significant contributions fields including engineering architecture law governance military language infrastructure comparing key differences philosophy art culture government science math shortly civilizations left lasting legacies associated philosophy art renowned engineering law governance</t>
+          <t>laws ruler 2 consuls steal government stop eachother senate prohibited engaging banking foreign trade</t>
         </is>
       </c>
       <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>3</v>
+      </c>
+      <c r="E42" t="n">
+        <v>7</v>
+      </c>
+      <c r="F42" t="n">
+        <v>7</v>
+      </c>
+      <c r="G42" t="n">
         <v>13</v>
       </c>
-      <c r="D42" t="n">
-        <v>9</v>
-      </c>
-      <c r="E42" t="n">
-        <v>13</v>
-      </c>
-      <c r="F42" t="n">
-        <v>12</v>
-      </c>
-      <c r="G42" t="n">
-        <v>15</v>
-      </c>
       <c r="H42" t="n">
-        <v>14.87897012500446</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>20210808608</v>
+        <v>20210808061</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>power division includes counselors senate assembles system country ruled objective</t>
+          <t>accused guilty proven guilty established 12 tables revolt plebs thought knew laws established modern law system called division power 3 parties guard despotism consuls 2 people military political head state enormous power senate things safeguard means ability veto s decision senate power unpaid served life found guilty advisor body consuls interest conflict means people power etc senate found guilty taken senate power corruption etc assemblies representative tribes people</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D43" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F43" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G43" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H43" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>20210808610</v>
-      </c>
-      <c r="B44" t="inlineStr"/>
+        <v>20210808044</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>lawyer judge prison suspects innocent guilty proved research previous judgement judgements</t>
+        </is>
+      </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F44" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G44" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H44" t="n">
-        <v>0</v>
+        <v>18.15373682851673</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>20210808612</v>
+        <v>20220808703</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>roads highways butterfield surgery tables julian calender search universe example moon earth calculate distance earth moon</t>
+          <t>advocaat system jury system prison system specific time</t>
         </is>
       </c>
       <c r="C45" t="n">
         <v>8</v>
       </c>
       <c r="D45" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F45" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G45" t="n">
         <v>14</v>
       </c>
       <c r="H45" t="n">
-        <v>5.899757610357249</v>
+        <v>18.43866113669333</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>20210808614</v>
+        <v>20210808033</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>aqueducts welfare newspaper bound books concrete julian calender</t>
+          <t>division power theatre manage people new government chose console separation power tem limits regular elections</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E46" t="n">
         <v>9</v>
       </c>
       <c r="F46" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G46" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H46" t="n">
-        <v>8.624239984852467</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>20210808615</v>
+        <v>20220808073</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>powerful laws instead bit similar</t>
+          <t>lawyer venice story jury giving verdict prison punish people future wanted fair system meet theatre plays debate community s problems bad possibilities plays life real life</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D47" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F47" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G47" t="n">
         <v>14</v>
       </c>
       <c r="H47" t="n">
-        <v>0</v>
+        <v>17.85657956764896</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>20210808616</v>
+        <v>20220808035</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>engineering agriculture military significant contributions development western civilization</t>
+          <t>introduce 3 things consuls senate assemblies consuls powerful organization government command army said political events senate free charge legal power t engage banking foreign trades conflict interest assemblies represent people</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E48" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F48" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G48" t="n">
         <v>14</v>
       </c>
       <c r="H48" t="n">
-        <v>10.33974754562162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>20220808001</v>
+        <v>20230808614</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>better military engineering improved science lot big highways deploy army quicker good trading better government system rules shouldn t rules punished</t>
+          <t>lawyer jury assembly accused innocent proven guilty</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D49" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E49" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F49" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G49" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H49" t="n">
-        <v>8.867312686149578</v>
+        <v>19.65799899268326</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>20220808002</v>
+        <v>20220808025</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>theatre shows closed public</t>
+          <t>accused innocent proven guilty judgment punishment based precedent</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D50" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F50" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G50" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H50" t="n">
-        <v>0</v>
+        <v>19.13030022685658</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>20220808005</v>
+        <v>20210808610</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>government society example theatres public military strong strong large empire studying practical generally military theoretical</t>
+          <t>humanity socialite</t>
         </is>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E51" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G51" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -1868,49 +1864,49 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>20220808006</v>
+        <v>20210808016</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>good military civil engineering established highways roads interested technology created modern laws system republic science important technology important science tool</t>
+          <t>checks balances legs actions formula system cognition extraordinary period republic vetoes separation powers term limits regular elections jus civil developed applied exclusively roman citizens type law jus genius developed applied foreigners</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D52" t="n">
         <v>8</v>
       </c>
       <c r="E52" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F52" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G52" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H52" t="n">
-        <v>13.41517576895199</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>20220808007</v>
+        <v>20230808618</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>bring republic world constitution simple writing rules known previous civilizations</t>
+          <t>democratic government like antic athena governments 3 things consults assemblies senate 2 consults consult power military etc senate doesn t power advice consults assemblies create new law twelve laws father rights lots highways gets lots money</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E53" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F53" t="n">
         <v>11</v>
@@ -1919,107 +1915,107 @@
         <v>15</v>
       </c>
       <c r="H53" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>20220808010</v>
+        <v>20230808004</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>law understand predict science nature developed law legal system creature highways structure</t>
+          <t>1 lawyer concept - story venice 2 trial credit jury concept assemblies consul generally listen jury says 3 suspect guilty trial decision prison keeps arrest trial</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D54" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E54" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F54" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G54" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H54" t="n">
-        <v>11.43582014911964</v>
+        <v>17.91478090863153</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>20220808013</v>
+        <v>20230808617</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>julian calendar difference work science engineering</t>
+          <t>innocent proven guilty lawyers translators lawyers senate councils</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D55" t="n">
         <v>3</v>
       </c>
       <c r="E55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G55" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H55" t="n">
-        <v>6.709959918628646</v>
+        <v>19.59520177453928</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>20220808014</v>
+        <v>20210808017</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>build new highways trade products want easier developed laws judge people</t>
+          <t>actually find lawyer jury prison system according roman mentality anybody nt prisioner proof evidence</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D56" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E56" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F56" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G56" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H56" t="n">
-        <v>9</v>
+        <v>14.0306192545827</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>20220808016</v>
+        <v>20220808041</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>invented roads primitive highways invented 12 tablets cure conflict interest making consumer assemblies senator</t>
+          <t>plebs think good law said writing law everbody trust established 12 tables idea 3 concepts jury prison lawyer thought person judgment innocent proven guilty thought laws consistent judgment punishment based precedent</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D57" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E57" t="n">
         <v>12</v>
@@ -2028,47 +2024,47 @@
         <v>12</v>
       </c>
       <c r="G57" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H57" t="n">
-        <v>15.91755914088441</v>
+        <v>6.796376481738273</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>20220808018</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>inventions found newspaper concrete julian julius calendar tables roman arches welfare biggest difference policy democracy suffered trying representative ways succeed</t>
-        </is>
-      </c>
+        <v>20220808033</v>
+      </c>
+      <c r="B58" t="inlineStr"/>
       <c r="C58" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E58" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G58" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H58" t="n">
-        <v>14.584824231048</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>20220808019</v>
-      </c>
-      <c r="B59" t="inlineStr"/>
+        <v>20220808052</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>lawyer jury prison everybody innocent proven guilty 12 rules</t>
+        </is>
+      </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
@@ -2082,133 +2078,131 @@
       <c r="G59" t="n">
         <v>0</v>
       </c>
-      <c r="H59" t="n">
-        <v>0</v>
-      </c>
+      <c r="H59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>20220808022</v>
+        <v>20220808616</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>julian calendar division power theatre gregorian calender divided power managed empire consuls assemblies senate</t>
+          <t>introduced written rules laws systematic approach leading empire</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F60" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G60" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H60" t="n">
-        <v>9.93486997559946</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>20220808023</v>
+        <v>20210808021</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>achievement include julian calendar battlefield medicine military system written laws division power greek s science philosophy rome focused things like ruling mechanism military advancements scientific progress little</t>
+          <t>consumes assembly senora</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D61" t="n">
         <v>5</v>
       </c>
       <c r="E61" t="n">
+        <v>5</v>
+      </c>
+      <c r="F61" t="n">
+        <v>7</v>
+      </c>
+      <c r="G61" t="n">
         <v>12</v>
       </c>
-      <c r="F61" t="n">
-        <v>11</v>
-      </c>
-      <c r="G61" t="n">
-        <v>16</v>
-      </c>
       <c r="H61" t="n">
-        <v>11.80150564141911</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>20220808024</v>
+        <v>20200808505</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>efficient travel network julian calendar news paper battlefield surgery difference military type roman legal system law ruler</t>
+          <t>roman law newspaper julian calendar elements surgery aqueduct criticizing government people</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E62" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G62" t="n">
         <v>16</v>
       </c>
       <c r="H62" t="n">
-        <v>12.53620564394753</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>20220808025</v>
+        <v>20230808623</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>built highways collesiums architecture places lived long years live like democratic fair effective think</t>
+          <t>introduced concept lawyers defends suspects court jurors jury gives verdict roma persons suspected crime imprisoned innocence proven</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D63" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E63" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F63" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G63" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H63" t="n">
-        <v>11.32480273718343</v>
+        <v>17.97375958901086</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>20220808026</v>
+        <v>20210808038</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>military important roman people constructed roads roman legions rapidly deployed military important travel network empire situation dramitaclly increased rome s influence power greek</t>
+          <t>develop legal laws 12 tablets basically laws introduces division power consuls senate assemblies forbidden senate s interfere banking trading conflict interest</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D64" t="n">
         <v>0</v>
@@ -2226,46 +2220,46 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>20220808028</v>
+        <v>20220808047</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>roma vast efficient travel network roma affected culture roma improving</t>
+          <t>julien schedule sunspots courts people controlling country sides king decision</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D65" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G65" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H65" t="n">
-        <v>9.900336372068272</v>
+        <v>17.63175858169411</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>20220808029</v>
+        <v>20220808039</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>contributions greece rome philosophy religion political legal institutions poetry drama means open - minded religious didn t questioned know</t>
+          <t>introduced main concepts lawyers</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D66" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E66" t="n">
         <v>9</v>
@@ -2277,44 +2271,48 @@
         <v>15</v>
       </c>
       <c r="H66" t="n">
-        <v>9.564179850880361</v>
+        <v>17.68042086590775</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>20220808032</v>
+        <v>20220808056</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>asked questions science interested laws rules law called division power philosophers interested government things</t>
+          <t>twelve tables established laws de lawyer punishment ıf somebody didnot obey tote rules punished laws prison murderer guilty arrest crime guilty proven everybody innocent jury verdict legal system rome judgmentsare longer hand kings priests plebs wanted twelve tables code laws venice story code laws consuls appointed popular assembly political military heads state 2 senate legal power held significant influence forbidden engage banking foreign trade conflict interest violation relationship based trust intrigues secret affairs 3 assemblies power pass law representatives tribes people extend</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D67" t="n">
         <v>8</v>
       </c>
       <c r="E67" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F67" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G67" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H67" t="n">
-        <v>11.57348231172666</v>
+        <v>6.186610504331682</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>20220808033</v>
-      </c>
-      <c r="B68" t="inlineStr"/>
+        <v>20220808032</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>lawyer jury prison person arrest accused innocent proven guilty</t>
+        </is>
+      </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D68" t="n">
         <v>0</v>
@@ -2328,355 +2326,355 @@
       <c r="G68" t="n">
         <v>0</v>
       </c>
-      <c r="H68" t="n">
-        <v>0</v>
-      </c>
+      <c r="H68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>20220808034</v>
+        <v>20220808043</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>good law established 12 tablets science explain nature</t>
+          <t>based distinction public law private law distinction time roman law actually foundations laws defending individual rights laid</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D69" t="n">
+        <v>8</v>
+      </c>
+      <c r="E69" t="n">
+        <v>15</v>
+      </c>
+      <c r="F69" t="n">
         <v>11</v>
       </c>
-      <c r="E69" t="n">
-        <v>12</v>
-      </c>
-      <c r="F69" t="n">
-        <v>13</v>
-      </c>
       <c r="G69" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H69" t="n">
-        <v>16.76123099209231</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>20220808035</v>
+        <v>20230808062</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>invented tables changed rules law introduced lawyer term roads highways time didn t happened conflict interest changed power judgment like consuls senate assemblies king power judgment judged judged want government power judgment wasn t wrong decisions</t>
+          <t>3 parts consuls heads state - putting laws - power veto - commanding army 2 senate selected populace attendance populace - judged guilty - conflicts interest 3 assemblies power pass law - heading people tribes - laws voted consuls closed assemblies don t right accept deny suggest</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D70" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E70" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G70" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H70" t="n">
-        <v>13.46379435605247</v>
+        <v>18.20811963173465</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>20220808037</v>
+        <v>20220808053</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>invented newspaper roads highways bound books julian calendars base difference developed science sciences developed develop technology</t>
+          <t>introduce law amp judgement system 12 tablet system 2 consult consults reject consult rome equal ruler system called conflict interest says consults trade banking purpose system fair law system</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D71" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E71" t="n">
+        <v>13</v>
+      </c>
+      <c r="F71" t="n">
         <v>12</v>
       </c>
-      <c r="F71" t="n">
-        <v>11</v>
-      </c>
       <c r="G71" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H71" t="n">
-        <v>12.09157279509073</v>
+        <v>3.766145759061934</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>20220808038</v>
+        <v>20200808504</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>legal system improving judgment division power important government roads highways military today important quote situation roads come roma newspaper reach population theatre theatre theatre government</t>
+          <t>law division power console senate roman acute s law system calendar newspaper thermometer elements</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E72" t="n">
         <v>12</v>
       </c>
       <c r="F72" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G72" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H72" t="n">
-        <v>13.5553671511432</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>20220808039</v>
+        <v>20220808045</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>known built highways roads arches tend expand hand worked science philosophy cement built arches published newspapers</t>
+          <t>didn t rule singular power king invented calculus legal concepts want define simple era people innocent prove quality</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E73" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F73" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G73" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H73" t="n">
-        <v>10.45076495755783</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>20220808041</v>
+        <v>20210808614</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>legal system law system idea called quit division power quit 3 instead king consuls senator assemblies theatre rome instance roman s theatre public protocol system theatre want public republic population voting power</t>
+          <t>consul new government appointed 2 counsels military police power responsible army lead sent consul stop s decision sent legal power serving advisory body engage banking foreign trade assembly create lows represented tribes extent general public</t>
         </is>
       </c>
       <c r="C74" t="n">
+        <v>0</v>
+      </c>
+      <c r="D74" t="n">
         <v>6</v>
       </c>
-      <c r="D74" t="n">
-        <v>7</v>
-      </c>
       <c r="E74" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F74" t="n">
         <v>8</v>
       </c>
       <c r="G74" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H74" t="n">
-        <v>11.2586197505618</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>20220808043</v>
+        <v>20200808008</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>roman people worked science far away mythology progressing based law system senate consuls like proggresings age</t>
+          <t>lawyer jury gives verdict accused person stays prison trial accused person innocent guilty proved</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D75" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E75" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G75" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H75" t="n">
-        <v>11.19778755458793</v>
+        <v>19.54272095256077</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>20220808044</v>
+        <v>20220808046</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>introduced modern law notions built roads highways introduced 12 tables law invented julian calender newspaper concrete roman arch bound books battlefield surgery welfare engineers interested finding rational answers questions science systematic approach tool practical tried understand predict observations engineering purposes</t>
+          <t>senator consult veto</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D76" t="n">
+        <v>3</v>
+      </c>
+      <c r="E76" t="n">
+        <v>6</v>
+      </c>
+      <c r="F76" t="n">
+        <v>6</v>
+      </c>
+      <c r="G76" t="n">
         <v>13</v>
       </c>
-      <c r="E76" t="n">
-        <v>15</v>
-      </c>
-      <c r="F76" t="n">
-        <v>14</v>
-      </c>
-      <c r="G76" t="n">
-        <v>17</v>
-      </c>
-      <c r="H76" t="inlineStr"/>
+      <c r="H76" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>20220808045</v>
+        <v>20230808061</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>walls highways highways involved network trade area law developed legal system creature built structures invent</t>
+          <t>invented law system power senate juries nation judge king conflict interests</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D77" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E77" t="n">
         <v>12</v>
       </c>
       <c r="F77" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G77" t="n">
         <v>15</v>
       </c>
       <c r="H77" t="n">
-        <v>12.76796982122946</v>
+        <v>16.29143674186393</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>20220808046</v>
+        <v>20210808048</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>roads highway newspaper supplement 1 supplement 2 describe nature science practice science</t>
+          <t>probably important civil right conflict interest important</t>
         </is>
       </c>
       <c r="C78" t="n">
+        <v>0</v>
+      </c>
+      <c r="D78" t="n">
+        <v>6</v>
+      </c>
+      <c r="E78" t="n">
+        <v>8</v>
+      </c>
+      <c r="F78" t="n">
+        <v>8</v>
+      </c>
+      <c r="G78" t="n">
         <v>13</v>
       </c>
-      <c r="D78" t="n">
-        <v>4</v>
-      </c>
-      <c r="E78" t="n">
-        <v>9</v>
-      </c>
-      <c r="F78" t="n">
-        <v>8</v>
-      </c>
-      <c r="G78" t="n">
-        <v>12</v>
-      </c>
       <c r="H78" t="n">
-        <v>6.825935047581178</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>20220808047</v>
+        <v>20220808028</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>court justice came discover discus self t courts lots product theory rejected court additionally court frightening killing science men free peaceful lots time thinking science</t>
+          <t>consuls senator assemblies accused innocent proven guilty roma</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D79" t="n">
         <v>4</v>
       </c>
       <c r="E79" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F79" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G79" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H79" t="n">
-        <v>5.692037450287549</v>
+        <v>18.71787950115239</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>20220808048</v>
+        <v>20220808066</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>law system calender system corrected old calendars leap year 100 years</t>
+          <t>lawyer jury prison</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D80" t="n">
         <v>4</v>
       </c>
       <c r="E80" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G80" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H80" t="n">
-        <v>7</v>
+        <v>19.54272095256077</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>20220808050</v>
+        <v>20210808056</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>accept think</t>
+          <t>layer jury prison 12 tables</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D81" t="n">
         <v>0</v>
@@ -2690,313 +2688,305 @@
       <c r="G81" t="n">
         <v>0</v>
       </c>
-      <c r="H81" t="n">
-        <v>0</v>
-      </c>
+      <c r="H81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>20220808051</v>
+        <v>20210808066</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>calendar improved calendar basic calendars unlike invented 3 calendar nowadays battlefield surgery invented new tools medicine roman aqueducts roman s population increasing need water built aqueducts build aqueducts roads roman s population increasing huge places improved roads population length roads main difference newspaper wanted record daily actions newspaper tablets rocks</t>
+          <t>democracy twelve table rules 12 table rules assemblies senate consult division power humanism democracy freedom philosophy - humanism play dash comedy tragedy br style color rob 36 36 36</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D82" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E82" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F82" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G82" t="n">
         <v>16</v>
       </c>
       <c r="H82" t="n">
-        <v>12.78739732991374</v>
+        <v>3.584485589041843</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>20220808052</v>
+        <v>20220808034</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>span style fantasize 24px aqueducts roman roads roman law concrete contribution aqueducts network water transportation famous roads leads rome genius engineering layered roads roads military trade legal system foundation modern legal procedures like jury lawyer prisons lastly method concrete making expert level considering today s standard science military purposes unlike science purely explain predict nature span</t>
+          <t>good law today rules</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E83" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F83" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G83" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H83" t="n">
-        <v>15.74880831403379</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>20220808053</v>
+        <v>20220808074</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>aqua way big roads battle surgery concrete especially army kind law system work ancient system worked rome</t>
+          <t>3 type system instead king consuls senate assemblies applied punishment judgment based previous situation</t>
         </is>
       </c>
       <c r="C84" t="n">
         <v>8</v>
       </c>
       <c r="D84" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E84" t="n">
         <v>12</v>
       </c>
       <c r="F84" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G84" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H84" t="n">
-        <v>13.32360297386126</v>
+        <v>17.16495505277223</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>20220808055</v>
+        <v>20220808067</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>like 12 table like small constitution julian calendar 12 months 30 days highways built military economy newspaper reaching people modern legal system division power theaters form audiences sitting randomly theaters masks actors theatre realistic</t>
+          <t>ruler t arbitrary judge democratic ways consulted senate</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D85" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F85" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G85" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H85" t="n">
-        <v>12.25119168596621</v>
+        <v>18.26250243495234</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>20220808056</v>
+        <v>20220808037</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>theater influence people outfor entertainment influenced theater soldier tradesmen systems law system</t>
+          <t>everybody clear guilty detected division power management society</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D86" t="n">
+        <v>5</v>
+      </c>
+      <c r="E86" t="n">
         <v>6</v>
       </c>
-      <c r="E86" t="n">
-        <v>8</v>
-      </c>
       <c r="F86" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G86" t="n">
-        <v>15</v>
-      </c>
-      <c r="H86" t="n">
-        <v>7</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="H86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>20220808057</v>
+        <v>20210808612</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>better structure military system create 12 tables 10 innovations chosen people theatre greek people theatre</t>
+          <t>lawyers jury verdict prison waited punishment accused innocent proven guilty</t>
         </is>
       </c>
       <c r="C87" t="n">
+        <v>20</v>
+      </c>
+      <c r="D87" t="n">
         <v>3</v>
       </c>
-      <c r="D87" t="n">
-        <v>8</v>
-      </c>
       <c r="E87" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F87" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G87" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H87" t="n">
-        <v>8</v>
+        <v>19.31217944760186</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>20220808058</v>
+        <v>20200808045</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>ancient observation theories explain nature weren t good engineering technological contribution civilization humanity course definitely t prominent quality advanced engineering constructed water arches dishes important quality constructing highways roads - created military purposes came important commerce republic concept ancient actually democratic countries differs republic</t>
+          <t>consuls senate assemblies people free prove guilty division power</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D88" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E88" t="n">
         <v>9</v>
       </c>
       <c r="F88" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G88" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H88" t="n">
-        <v>10.85874681295927</v>
+        <v>18.20239911273036</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>20220808059</v>
+        <v>20210808616</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>good civil military engineering roads legions roads important economic power road exits rome modern judgment system didn t</t>
+          <t>significant contributions development legal concepts systems lasting impact modern legal principles practices modern legal concepts introduced civil rights contracts property corporations</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E89" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F89" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G89" t="n">
         <v>16</v>
       </c>
       <c r="H89" t="n">
-        <v>10.1177127217492</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>20220808060</v>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>expanding empire s transport network boosted empire s authority impact 12 table laws understand 12 table laws king</t>
-        </is>
-      </c>
+        <v>20210808076</v>
+      </c>
+      <c r="B90" t="inlineStr"/>
       <c r="C90" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D90" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E90" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G90" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H90" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>20220808062</v>
+        <v>20220808604</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>science understand nature observation prediction learned proofs stated axioms</t>
+          <t>laws mentioned guilty prove guilty systems introducing lawyer prison jury nowadays</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D91" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E91" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
         <v>9</v>
       </c>
       <c r="G91" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H91" t="n">
-        <v>8.305772820681133</v>
+        <v>17.62603806269005</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>20220808063</v>
+        <v>20220808022</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>copy</t>
+          <t>calender roads highways archer concrete</t>
         </is>
       </c>
       <c r="C92" t="n">
         <v>0</v>
       </c>
       <c r="D92" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E92" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F92" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G92" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H92" t="n">
         <v>0</v>
@@ -3004,291 +2994,295 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>20220808066</v>
+        <v>20220808705</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>roman roads aqueducts concrete roman law director 3 people instead director like senator consuls people choose roman roads military concrete invented building instrecture</t>
+          <t>lawyer prison people jury decide people</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D93" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E93" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G93" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H93" t="n">
-        <v>11.49164771267388</v>
+        <v>18.62054035743861</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>20220808067</v>
+        <v>20220808010</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>science practical tool science creating useful concrete newspaper systematic observation try explain nature deductions try prove theory deduction relativism cumulative</t>
+          <t>walls highways introduce law person innocent guilty proven understand law works assembles senate law creature built nice structures developed legal system important science</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D94" t="n">
         <v>7</v>
       </c>
       <c r="E94" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F94" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G94" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H94" t="n">
-        <v>10.40057974159549</v>
+        <v>16.11527804012271</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>20220808069</v>
+        <v>20210808042</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>engineering agriculture philosophy religion poetry drama arches roads highways bound book theatre based fun greek theatre based reach people science relieve anxiety knowledge democratic republic</t>
+          <t>introduce prison system jury system accused innocent proven guilty</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D95" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E95" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G95" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H95" t="n">
-        <v>9.243674942123606</v>
+        <v>18.84727789991916</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>20220808071</v>
+        <v>20230808020</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>achieved good agriculture cinematic science cumulative progressive</t>
+          <t>repeating power conflict interest</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E96" t="n">
         <v>7</v>
       </c>
       <c r="F96" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G96" t="n">
         <v>13</v>
       </c>
       <c r="H96" t="n">
-        <v>6.917318462043403</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>20220808072</v>
+        <v>20220808044</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>improved civil military engineering efficient roads provide center trade</t>
+          <t>lawyer jury prison person arrest trial accused innocent proven guilty</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D97" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G97" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H97" t="n">
-        <v>10.10671958350954</v>
+        <v>19.19499942623997</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>20220808073</v>
+        <v>20230808608</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>aqueducts news paper bond books roads highways tables difference ended progress science paid attention best civil engineering military engineering protect empire</t>
+          <t>separation forces innocent proven guilty real estate laws ownership lands senate system senate elections representation common folk prevention trading certain law related people</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D98" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E98" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G98" t="n">
         <v>15</v>
       </c>
       <c r="H98" t="n">
-        <v>11.30880496652415</v>
+        <v>18.02624041098937</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>20220808074</v>
+        <v>20220808007</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>good civil military engineering enormous economics highways roads trade science practical tool strictly deductive proof based stated axioms observation theory theory looking nature things happened like</t>
+          <t>division power republic democracy</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D99" t="n">
         <v>6</v>
       </c>
       <c r="E99" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F99" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G99" t="n">
         <v>14</v>
       </c>
       <c r="H99" t="n">
-        <v>10.33974754562162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>20220808076</v>
+        <v>20200808038</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>fi stay calendar prove julia calendar gregory calendar secondly bui ld lots hi way 12 table</t>
+          <t>judgement punishment based precedent person observation trial persons innocent proven guilty jury gives verdict</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D100" t="n">
         <v>5</v>
       </c>
       <c r="E100" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F100" t="n">
         <v>9</v>
       </c>
       <c r="G100" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H100" t="n">
-        <v>9.564179850880361</v>
+        <v>18.55584115805523</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>20220808077</v>
+        <v>20220808072</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>improved medicine better things found roads rome unlike greece idiom quit roads leads rome quit comes roman months greece</t>
+          <t>instead king 3 parties consult consumes safety vote seneca military power assemblies representative people pass law</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D101" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E101" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F101" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G101" t="n">
         <v>14</v>
       </c>
       <c r="H101" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>20220808504</v>
+        <v>20190808035</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>roman innovations concrete newspaper bound boys julian calendar ıs worked science far away methods progress based law system</t>
+          <t>division power concept parts include council senate assembly</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D102" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E102" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F102" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G102" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H102" t="n">
-        <v>10.68943526726181</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>20220808601</v>
-      </c>
-      <c r="B103" t="inlineStr"/>
+        <v>20220808057</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>equality accuse innocent given proven guilty 12 tables equality conflict interest shouldn t change old rules create division power</t>
+        </is>
+      </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D103" t="n">
         <v>0</v>
@@ -3302,248 +3296,246 @@
       <c r="G103" t="n">
         <v>0</v>
       </c>
-      <c r="H103" t="n">
-        <v>0</v>
-      </c>
+      <c r="H103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>20220808604</v>
+        <v>20230808066</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>better example law system power division consult senator assemblies example military military perfectlier care military spending</t>
+          <t>lawyer - venice story jury - judge verdict prison - person arrest trial accused innocent proven guilty</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D104" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E104" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F104" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G104" t="n">
         <v>14</v>
       </c>
       <c r="H104" t="n">
-        <v>8</v>
+        <v>18.43675915545415</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>20220808606</v>
+        <v>20230808055</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>important science universal continuing</t>
+          <t>modern concepts introduce lawyer jury prison idea suspect consider innocent proven guilty</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D105" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E105" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F105" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G105" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H105" t="n">
-        <v>6.466525600676592</v>
+        <v>18.08903762913335</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>20220808607</v>
+        <v>20210808006</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>jules calender roads military deployment difference democratic law enforcement science improve military things science observe nature understand</t>
+          <t>jury verdict prison person arrest trial corpus juries include accused innocent proven guilty judgment punishments based precedent rulings previous judges juries developed complex legal system influenced modern laws city - state democracies didnot create united legal system like law people theatre allow people theatre athenian ancient city democracy drama tragedy roman science invented</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D106" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E106" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F106" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G106" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H106" t="n">
-        <v>11.0149448084382</v>
+        <v>6.796376481738273</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>20220808608</v>
+        <v>20230808075</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>agriculture cumulative progressive abstraction predict</t>
+          <t>plebs revolt twelve tables established unlike didn t rule singular power like king invented consumes senator assemblies consumes 2 supreme power army state veto decision pressure single ruler division power senator legal power serving life time found guilty forbidden senator engage bank foreign trade conflict interests assemblies presenting tribe people people power voting suspect innocent proven guilty trial</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D107" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E107" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F107" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G107" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H107" t="n">
-        <v>6.917318462043403</v>
+        <v>16.52769876582691</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>20220808610</v>
+        <v>20200808015</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>important roads highways arches concrete julien calendar better civil engineering military engineering roads highways lead economical power world saying quit roads leads rome quit</t>
+          <t>wanted create good community lot modern legal concepts example bring law</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D108" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E108" t="n">
+        <v>13</v>
+      </c>
+      <c r="F108" t="n">
         <v>11</v>
       </c>
-      <c r="F108" t="n">
-        <v>10</v>
-      </c>
       <c r="G108" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H108" t="n">
-        <v>10.52259029177136</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>20220808616</v>
+        <v>20200808003</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>science practical tool resulted improve technological engineering fields contribution science contribution technology catapults throw huge rock enemy ships roman s inventions came military motivation hand wanted prove knowledge knew practically modeling maths wanted strictly deductive proofs axioms understand clearly tried developed approaches scientific works</t>
+          <t>lawyer - venice story jury verdict prison person arrest trial corpus juries included modern legal concepts liquor accused innocent proven guilty duo judgment punishments based precedent rulings previous judges juries</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D109" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E109" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F109" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G109" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H109" t="n">
-        <v>12.31357340264074</v>
+        <v>16.23436004272379</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>20220808617</v>
+        <v>20220808058</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>julian calender roads highways newspaper tables roads highways legions thanks increase fast manage roman division interest mean consults senate assembles system civilians choose manage</t>
+          <t>legal modern concepts introduced lawyer concept - actually form translator translation problems city venice turning reason venice port city lots communication problems created concept solve problem jury concept - jury concepts defines group people ve judged accused people judge court similar concept jury lots country today concept assuming innocent guilt proved 4 - concept type sample determination example let s 2 files similar second affected s result</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D110" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E110" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F110" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G110" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H110" t="n">
-        <v>12.53620564394753</v>
+        <v>16.41051874446501</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>20220808703</v>
+        <v>20220808018</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>military trade roads highways military state power legal laws democracy senate consuls assemblies</t>
+          <t>democracy freedom representation didn t accept monarchy instead king representation rome consumes senate assemblies thought accused innocent proven guilty</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D111" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E111" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F111" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G111" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H111" t="n">
-        <v>12.53620564394753</v>
+        <v>18.55393917681605</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>20220808705</v>
+        <v>20220808001</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>division power division power consult senator assemblies concept lawyer jury prison roma theater open public unlike greek roma theater classification roma theater sitting agreement military engineering theater entertainment greek theater political</t>
+          <t>introduced 3 concepts modern legal jury verdict punishment lead crimes thing lawyer thing prison arrest believed accused innocent proven guilty</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D112" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E112" t="n">
         <v>9</v>
@@ -3555,135 +3547,135 @@
         <v>15</v>
       </c>
       <c r="H112" t="n">
-        <v>10.0565343675472</v>
+        <v>18.02624041098937</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>20220808706</v>
+        <v>20220808077</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>copy</t>
+          <t>division power consuls senate assemblies conflict interest idiom innocent proven guilty voting system legal laws 12 tablets</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D113" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E113" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F113" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G113" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H113" t="n">
-        <v>0</v>
+        <v>7.182188886828429</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>20230808004</v>
+        <v>20210808005</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>observation support theories explain nature good engineering democratically things builds network ways developed legal system consul senate assemblies consul decision military political events senate forbidden engage banking foreign trade assemblies power pass law representatives people extend</t>
+          <t>democracy freedom instead kings 3 democracy rules consuls senator assemblies consuls chosen new king number power broad found solution problem electing 2 consuls consul veto decision senator senator responsibilities found guilty private public case assemblies power stronger laws thought accused innocent found guilty</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D114" t="n">
         <v>5</v>
       </c>
       <c r="E114" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F114" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G114" t="n">
         <v>15</v>
       </c>
       <c r="H114" t="n">
-        <v>10.81645044985731</v>
+        <v>17.79569890603046</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>20230808010</v>
+        <v>20200808805</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>focused expanding military building roads highways focused science philosophy cement built arches published newspapers books schools didn t advanced buildings teacher thought religious important close democracy differently tables trials didn t legal system</t>
+          <t>- lawyer - prison person arrest trial -</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D115" t="n">
         <v>5</v>
       </c>
       <c r="E115" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F115" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G115" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H115" t="n">
-        <v>8.640590553095411</v>
+        <v>19.42554093119887</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>20230808020</v>
+        <v>20190808021</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>complicit inference separate power moon system</t>
+          <t>introduced 12 tables 12 tables 12 legal rules introduced concepts judge passed verdicts jury people listening giving opinions cases prisons built house accused people trials</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D116" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E116" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F116" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G116" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H116" t="n">
-        <v>0</v>
+        <v>3.386916982471849</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>20230808049</v>
+        <v>20220808606</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>center money travel thanks highways safety network great architecture ideas jury lawyer jails guilty people arrest developed division powers consuls 2 number head states senate formal power power important advisor consuls assemblies representatives great groups people forbidden engage banking relation rich people conflict interest improve science technology huge improvements technology architecture</t>
+          <t>introduced social science concepts improved democracy</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D117" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E117" t="n">
         <v>10</v>
@@ -3695,210 +3687,210 @@
         <v>15</v>
       </c>
       <c r="H117" t="n">
-        <v>9.858040008966309</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>20230808055</v>
+        <v>20200808063</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>build wast efficient road network great enormous architecture improved battle surgery difference develop science better engineers</t>
+          <t>citizen law</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D118" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E118" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F118" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G118" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H118" t="n">
-        <v>10.21773699544575</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>20230808061</v>
+        <v>20220808005</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>invented technologies civil engineering military engineering contribute science influence greek teacher develops huge teachers</t>
+          <t>law distinct power distinction public private law looking precedent church</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D119" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E119" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F119" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G119" t="n">
         <v>14</v>
       </c>
       <c r="H119" t="n">
-        <v>8.723502928907111</v>
+        <v>17.9832986457798</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>20230808062</v>
+        <v>20220808051</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>specific things division power military defence industry travel network big populace contains 36 country research science inventions rome tables juries corpus civilise aqueducts highways roads newspaper welfare concrete</t>
+          <t>lawyer jury prison guilty prove guilty</t>
         </is>
       </c>
       <c r="C120" t="n">
         <v>20</v>
       </c>
       <c r="D120" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E120" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F120" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G120" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H120" t="n">
-        <v>13.32360297386126</v>
+        <v>19.3064589285978</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>20230808066</v>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>tables - laws property divorce welfare newspaper - stones posted trafficked areas julian calender - 365 1 4 days caused shift seasons aqueduct battlefield surgery roads highways roman arches - buildings legal system concepts trafficked network highways powerful</t>
-        </is>
-      </c>
+        <v>20220808608</v>
+      </c>
+      <c r="B121" t="inlineStr"/>
       <c r="C121" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D121" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E121" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F121" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G121" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H121" t="n">
-        <v>15.37222156096174</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>20230808070</v>
+        <v>20220808060</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>powerful civilizations center world time king decided works fast rules laws king decided punishments people lots improvements established table rules act according expansion military overspending economic troubles slave work political instability continued bad accept existing situation questioned preferred evidence - based method theories observations</t>
+          <t>separated manage empire s categories consults people interested soldier work political work assemblies public choosed represented public</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D122" t="n">
         <v>7</v>
       </c>
       <c r="E122" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F122" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G122" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H122" t="n">
-        <v>11.3856349331573</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>20230808075</v>
+        <v>20220808026</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>civil military engineering roads highways legions deployed instantly makes trade easy improves economy roads leads rome law rules improved consumes senator assemblies newspapers construct aquebelt books parts battlefield surgery</t>
+          <t>people equal rome laws people consuls senate assemblies people consult - government changing senate changed elected populace appointed popular assembly consuls military political supreme power commanding army precedes senate ability vote s decision senate - legal power power influence serving advisory body consult later emperor individuals unpaid served life forbidden engage banking trading crossroads assemblies - representative people tribe extend elected officials representative bodies</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D123" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E123" t="n">
         <v>11</v>
       </c>
       <c r="F123" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G123" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H123" t="n">
-        <v>11.44646712913116</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>20230808077</v>
+        <v>20230808049</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>makes 12 table law roads highways compass bound books battle surgery approach law science</t>
+          <t>introduced jury judge people lawyer protect persons rights jails guilty people arrest improved idea innocent proven 12 tables basically mainly modern day</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D124" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E124" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F124" t="n">
         <v>12</v>
       </c>
       <c r="G124" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H124" t="n">
-        <v>16.58155775882484</v>
+        <v>6.390762739402524</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>20230808602</v>
-      </c>
-      <c r="B125" t="inlineStr"/>
+        <v>20210808604</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>12 modern legal concepts introduce</t>
+        </is>
+      </c>
       <c r="C125" t="n">
         <v>0</v>
       </c>
@@ -3920,127 +3912,127 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>20230808608</v>
+        <v>20220808002</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>similar modern law area calculations calendars separation forces innocent proven guilty philosophy architecture geometry mathematics action wise theoretical actual practical lot work theorized pretty based terms law litigation great trade soldier great terms strategy training</t>
+          <t>predicting 12 animal war situation law rules people rules statements</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D126" t="n">
         <v>7</v>
       </c>
       <c r="E126" t="n">
+        <v>10</v>
+      </c>
+      <c r="F126" t="n">
         <v>12</v>
       </c>
-      <c r="F126" t="n">
-        <v>9</v>
-      </c>
       <c r="G126" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H126" t="n">
-        <v>11.30880496652415</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>20230808609</v>
+        <v>20200808062</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>copy</t>
+          <t>invented 12 tablets fundamental modern law separation powers fundement democracy jail judge jury concepts judge people necessary</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D127" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E127" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F127" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="G127" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H127" t="n">
-        <v>0</v>
+        <v>1.365482351037776</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>20230808611</v>
+        <v>20230808615</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>concrete aqueducts improved architecture created newspaper created table created legal system didn t</t>
+          <t>wrote laws tablet order avoid confusions subjective decisions ruler regarded accused persons innocent proven guilty court similar today</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D128" t="n">
         <v>6</v>
       </c>
       <c r="E128" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F128" t="n">
         <v>8</v>
       </c>
       <c r="G128" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H128" t="n">
-        <v>10.53323727178289</v>
+        <v>17.33079735834776</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>20230808614</v>
+        <v>20220808062</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>didn t contribute science improved technology invented roads military purposes provided economic advantage successful republic history developed law system similar system today advanced architecture built aqueducts roman arches</t>
+          <t>laws sort elections columns theatre plebs effect isan government country given political powers plebs</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D129" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E129" t="n">
         <v>11</v>
       </c>
       <c r="F129" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G129" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H129" t="n">
-        <v>10.95411261246433</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>20230808615</v>
+        <v>20220808055</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>capable engineers interested theory like build roads structures inventions news paper battlefield surgery cement aqueducts welfare etc</t>
+          <t>lawyers search past cases helping people accused juries discuss cases find result model called precedent means juries look past similar cases comment system gave chance objective cases</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D130" t="n">
         <v>8</v>
@@ -4052,122 +4044,122 @@
         <v>10</v>
       </c>
       <c r="G130" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H130" t="n">
-        <v>10.58842712016485</v>
+        <v>16.63915826818473</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>20230808617</v>
+        <v>20210808065</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>great roads laws 12 table science understand nature wanted theorize facts science improve military need etc</t>
+          <t>protected private property rights quilted fundamentals modern law established innocent guilt proved concept</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D131" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E131" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F131" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G131" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H131" t="n">
-        <v>15.6663674549182</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>20230808618</v>
+        <v>20200808020</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>democracy like tragedy theatre greek body tragedy theatre equal roma everybody aren t equal n roma people loyal highways power economy highways information explain nature don t create engineering science engineering powerful weapons laws father rights etc newspaper lots build example bridges</t>
+          <t>innocence prove guilty twelve table laws corpus juries civilise consults senator assembling senator legal power assembling pass laws</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D132" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E132" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F132" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G132" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H132" t="n">
-        <v>9.010646980011526</v>
+        <v>5.187139221140021</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>20230808621</v>
+        <v>20220808038</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>invent road structures newspaper concrete entertainment theatre roman establish tables technics wanted strictly detective proof based stated axioms wanted real reason review theatre example theatre entertainment access improve democracy people join theatre theatre public</t>
+          <t>plebs thought unfair way legal system system lawyers juries prisons prisons place keeping people proven guilty 12 tables table written document judgment</t>
         </is>
       </c>
       <c r="C133" t="n">
         <v>20</v>
       </c>
       <c r="D133" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E133" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F133" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G133" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H133" t="n">
-        <v>14.111000303775</v>
+        <v>17.21551931822504</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>20230808623</v>
+        <v>20200808072</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>difference purpose science seek informations explains nature laws observed nature categorized predicted science practical especially engineering built roads water belts invented concrete newspapers improved battle surgery built sewer system cities</t>
+          <t>battlefield surgery newspaper twelve 12 tablets introduce kind modern legal concepts consuls senate assemblies</t>
         </is>
       </c>
       <c r="C134" t="n">
+        <v>8</v>
+      </c>
+      <c r="D134" t="n">
+        <v>12</v>
+      </c>
+      <c r="E134" t="n">
+        <v>14</v>
+      </c>
+      <c r="F134" t="n">
+        <v>14</v>
+      </c>
+      <c r="G134" t="n">
         <v>17</v>
       </c>
-      <c r="D134" t="n">
-        <v>9</v>
-      </c>
-      <c r="E134" t="n">
-        <v>13</v>
-      </c>
-      <c r="F134" t="n">
-        <v>11</v>
-      </c>
-      <c r="G134" t="n">
-        <v>14</v>
-      </c>
       <c r="H134" t="n">
-        <v>13.0815432238702</v>
+        <v>0.5740562036110957</v>
       </c>
     </row>
   </sheetData>
@@ -4181,7 +4173,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4208,66 +4200,53 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>20220808002</v>
+        <v>20210808048</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>theatre shows closed public</t>
+          <t>probably important civil right conflict interest important</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>20210808614</v>
+        <v>20220808005</v>
       </c>
       <c r="B3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>aqueducts welfare newspaper bound books concrete julian calender</t>
+          <t>law distinct power distinction public private law looking precedent church</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>20220808024</v>
+        <v>20190808021</v>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>efficient travel network julian calendar news paper battlefield surgery difference military type roman legal system law ruler</t>
+          <t>introduced 12 tables 12 tables 12 legal rules introduced concepts judge passed verdicts jury people listening giving opinions cases prisons built house accused people trials</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>20210808061</v>
+        <v>20220808052</v>
       </c>
       <c r="B5" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>established calendar established modern legal system good travel roadways highways good travel network grew economy science practical tool understand explain nature</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>20230808049</v>
-      </c>
-      <c r="B6" t="n">
-        <v>20</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>center money travel thanks highways safety network great architecture ideas jury lawyer jails guilty people arrest developed division powers consuls 2 number head states senate formal power power important advisor consuls assemblies representatives great groups people forbidden engage banking relation rich people conflict interest improve science technology huge improvements technology architecture</t>
+          <t>lawyer jury prison everybody innocent proven guilty 12 rules</t>
         </is>
       </c>
     </row>

</xml_diff>